<commit_message>
added layout notes to power sheet
</commit_message>
<xml_diff>
--- a/bici-pcb/Project Outputs for bici-pcb/bici-pcb.xlsx
+++ b/bici-pcb/Project Outputs for bici-pcb/bici-pcb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truth\OneDrive\Desktop\ACADEMICS\ENGN1650\engn1650-bici-pcb\bici-pcb\Project Outputs for bici-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D974005-7A05-4DF0-825E-585609F539CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A2AD5AF-3D97-45D2-A18A-D3D6F9AA69CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{A065C265-92BD-47E0-9912-ED16324AE730}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{BC0331EA-B744-437A-A090-AACE7A043FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="bici-pcb" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Supplier 1</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -353,7 +350,7 @@
     <t>RES SMD 0 OHM JUMPER 1/10W 0603</t>
   </si>
   <si>
-    <t>R7, R8, R9, R10</t>
+    <t>R7, R8, R9, R10, R11</t>
   </si>
   <si>
     <t>P0.0GCT-ND</t>
@@ -362,19 +359,19 @@
     <t>0</t>
   </si>
   <si>
-    <t>ERJ-3EKF60R4V</t>
-  </si>
-  <si>
-    <t>RES SMD 60.4 OHM 1% 1/10W 0603</t>
+    <t>ERJ-3EKF1200V</t>
+  </si>
+  <si>
+    <t>RES SMD 120 OHM 1% 1/10W 0603</t>
   </si>
   <si>
     <t>R201, R202, R203, R204, R205, R206, R207, R208, R209, R210, R211, R212, R213, R214</t>
   </si>
   <si>
-    <t>P60.4HCT-ND</t>
-  </si>
-  <si>
-    <t>60.4</t>
+    <t>P120HCT-ND</t>
+  </si>
+  <si>
+    <t>120</t>
   </si>
   <si>
     <t>ERJ-3EKF1002V</t>
@@ -923,8 +920,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30C92E8-E126-41A8-98B1-99E384FF5C2E}">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8423E8D4-26C9-44CC-AABF-637ED4E6E005}">
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -932,11 +929,10 @@
   <cols>
     <col min="1" max="3" width="15.3125" customWidth="1"/>
     <col min="4" max="4" width="10.15625" customWidth="1"/>
-    <col min="5" max="5" width="11.3671875" customWidth="1"/>
-    <col min="6" max="11" width="15.3125" customWidth="1"/>
+    <col min="5" max="10" width="15.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -967,29 +963,28 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>15</v>
@@ -1000,313 +995,303 @@
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D3" s="1">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="1">
         <v>5</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D7" s="1">
         <v>15</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1"/>
+      <c r="J7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="F9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="F10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="F12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>72</v>
@@ -1314,516 +1299,497 @@
       <c r="J12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="F13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>84</v>
       </c>
       <c r="J14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="F15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>90</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>95</v>
       </c>
       <c r="J16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="D17" s="1">
         <v>3</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="F17" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>100</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="1">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D18" s="1">
-        <v>4</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>105</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="1">
+        <v>14</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D19" s="1">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>110</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="D20" s="1">
         <v>6</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>115</v>
       </c>
       <c r="J20" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="F21" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>117</v>
+        <v>14</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>120</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="F22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="F23" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="1"/>
+      <c r="J23" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="F24" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="1"/>
+      <c r="J24" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="F25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="1"/>
+      <c r="J25" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="F26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="1"/>
+      <c r="J26" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="2" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="F27" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="1"/>
+      <c r="J27" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="F28" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="1"/>
+      <c r="J28" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exported bom and pdf of schematics
</commit_message>
<xml_diff>
--- a/bici-pcb/Project Outputs for bici-pcb/bici-pcb.xlsx
+++ b/bici-pcb/Project Outputs for bici-pcb/bici-pcb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truth\OneDrive\Desktop\ACADEMICS\ENGN1650\engn1650-bici-pcb\bici-pcb\Project Outputs for bici-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A2AD5AF-3D97-45D2-A18A-D3D6F9AA69CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65603B8D-F45B-4D9A-979D-B609408BFEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{BC0331EA-B744-437A-A090-AACE7A043FFF}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{FEA62213-A3F7-4A31-BFC2-CC4ECA34B1D0}"/>
   </bookViews>
   <sheets>
     <sheet name="bici-pcb" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
     <t>CAP CER 0.1UF 6.3V X7R 0603</t>
   </si>
   <si>
-    <t>C101, C402, C403, C404, C405</t>
+    <t>C101, C201, C202, C402, C403, C404, C405</t>
   </si>
   <si>
     <t>478-KGM15AR70J104JTCT-ND</t>
@@ -920,7 +920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8423E8D4-26C9-44CC-AABF-637ED4E6E005}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C16B119-2AC5-4B3F-98F1-E617E2E9BDDE}">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1039,7 +1039,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
exported BOM with changes
</commit_message>
<xml_diff>
--- a/bici-pcb/Project Outputs for bici-pcb/bici-pcb.xlsx
+++ b/bici-pcb/Project Outputs for bici-pcb/bici-pcb.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truth\OneDrive\Desktop\ACADEMICS\ENGN1650\engn1650-bici-pcb\bici-pcb\Project Outputs for bici-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CD3A6F2-6F7A-4AB4-9872-00254F77AC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE3A0EAB-D94A-4D67-869E-9186BB8FEF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{2C7AD2E0-6C97-4485-9083-9C9EA94C82E7}"/>
+    <workbookView xWindow="2808" yWindow="2808" windowWidth="17280" windowHeight="10134" xr2:uid="{C44DEFDD-B10F-4633-A67B-5CDC7B39C587}"/>
   </bookViews>
   <sheets>
     <sheet name="bici-pcb" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'bici-pcb'!$1:$1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="168">
   <si>
     <t>Name</t>
   </si>
@@ -95,10 +92,10 @@
     <t>0603</t>
   </si>
   <si>
-    <t>GRM188R60J106ME47D</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 6.3V X5R 0603</t>
+    <t>GRM188R61A106ME69D</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V X5R 0603</t>
   </si>
   <si>
     <t>C3, C4, C5</t>
@@ -107,10 +104,10 @@
     <t>Murata Electronics</t>
   </si>
   <si>
-    <t>490-3896-1-ND</t>
-  </si>
-  <si>
-    <t>10uF 6.3V</t>
+    <t>490-10475-1-ND</t>
+  </si>
+  <si>
+    <t>10 uF 10 V</t>
   </si>
   <si>
     <t>KGM15AR70J104JT</t>
@@ -119,7 +116,7 @@
     <t>CAP CER 0.1UF 6.3V X7R 0603</t>
   </si>
   <si>
-    <t>C101, C201, C202, C402, C403, C404, C405</t>
+    <t>C6, C101, C201, C202, C402, C403, C404, C405</t>
   </si>
   <si>
     <t>KYOCERA AVX</t>
@@ -179,6 +176,24 @@
     <t>4-PLCC</t>
   </si>
   <si>
+    <t>SDR08C04LP3-7B</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTK 4V 80MA X3DFN06032</t>
+  </si>
+  <si>
+    <t>D301, D302</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>31-SDR08C04LP3-7BCT-ND</t>
+  </si>
+  <si>
+    <t>0201</t>
+  </si>
+  <si>
     <t>AP3216ID</t>
   </si>
   <si>
@@ -329,19 +344,19 @@
     <t>2k</t>
   </si>
   <si>
-    <t>ERJ-3EKF1004V</t>
-  </si>
-  <si>
-    <t>RES SMD 1M OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R5, R6, R402</t>
-  </si>
-  <si>
-    <t>P1.00MHCT-ND</t>
-  </si>
-  <si>
-    <t>1M</t>
+    <t>RT0603BRD0750KL</t>
+  </si>
+  <si>
+    <t>RES 50K OHM 0.1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <t>13-RT0603BRD0750KLCT-ND</t>
+  </si>
+  <si>
+    <t>50k</t>
   </si>
   <si>
     <t>ERJ-3GEY0R00V</t>
@@ -350,7 +365,7 @@
     <t>RES SMD 0 OHM JUMPER 1/10W 0603</t>
   </si>
   <si>
-    <t>R7, R8, R9, R10, R11</t>
+    <t>R10, R11</t>
   </si>
   <si>
     <t>P0.0GCT-ND</t>
@@ -380,7 +395,7 @@
     <t>RES SMD 10K OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>R215, R216, R301, R303, R403, R404</t>
+    <t>R215, R216, R301, R303, R402, R404</t>
   </si>
   <si>
     <t>P10.0KHCT-ND</t>
@@ -389,21 +404,24 @@
     <t>10k</t>
   </si>
   <si>
-    <t>ERJ-3EKF11R0V</t>
-  </si>
-  <si>
-    <t>RES SMD 11 OHM 1% 1/10W 0603</t>
+    <t>ERJ-P06J110V</t>
+  </si>
+  <si>
+    <t>RES SMD 11 OHM 5% 1/2W 0805</t>
   </si>
   <si>
     <t>R302, R304</t>
   </si>
   <si>
-    <t>P11.0HCT-ND</t>
+    <t>P11ADCT-ND</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
+    <t>0805</t>
+  </si>
+  <si>
     <t>SLW-864574-5A-RA-N-D</t>
   </si>
   <si>
@@ -498,9 +516,6 @@
   </si>
   <si>
     <t>U301, U302</t>
-  </si>
-  <si>
-    <t>Diodes Incorporated</t>
   </si>
   <si>
     <t>DMG1012UW-7DICT-ND</t>
@@ -920,8 +935,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2150D750-15CD-4E4B-A8A1-C69239AC1EBD}">
-  <dimension ref="A1:J28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1338B1-C7CC-467C-88F0-7C518FEC3836}">
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1039,7 +1054,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>27</v>
@@ -1165,7 +1180,7 @@
         <v>48</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>49</v>
@@ -1210,155 +1225,153 @@
         <v>56</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="1">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
@@ -1403,10 +1416,10 @@
         <v>93</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>91</v>
@@ -1415,10 +1428,10 @@
         <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>17</v>
@@ -1426,31 +1439,31 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="1">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="G17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>17</v>
@@ -1458,31 +1471,31 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D18" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>17</v>
@@ -1490,31 +1503,31 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="1">
-        <v>14</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="G19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>17</v>
@@ -1522,31 +1535,31 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="1">
+        <v>14</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="1">
-        <v>6</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="G20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>17</v>
@@ -1554,31 +1567,31 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="G21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>17</v>
@@ -1586,22 +1599,22 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>14</v>
@@ -1609,177 +1622,179 @@
       <c r="H22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="I22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="J23" s="2" t="s">
-        <v>131</v>
-      </c>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="G26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>14</v>
@@ -1792,8 +1807,37 @@
         <v>161</v>
       </c>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nvm this actually updated all the params for all components (following vendor updates for some)
</commit_message>
<xml_diff>
--- a/bici-pcb/Project Outputs for bici-pcb/bici-pcb.xlsx
+++ b/bici-pcb/Project Outputs for bici-pcb/bici-pcb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truth\OneDrive\Desktop\ACADEMICS\ENGN1650\engn1650-bici-pcb\bici-pcb\Project Outputs for bici-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE3A0EAB-D94A-4D67-869E-9186BB8FEF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{85043DCA-A5A7-4381-AF0C-03A3EC3029D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="2808" windowWidth="17280" windowHeight="10134" xr2:uid="{C44DEFDD-B10F-4633-A67B-5CDC7B39C587}"/>
+    <workbookView xWindow="2808" yWindow="2808" windowWidth="17280" windowHeight="10134" xr2:uid="{D5D973EB-1224-46A1-97CA-BD7A8676D3D4}"/>
   </bookViews>
   <sheets>
     <sheet name="bici-pcb" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="169">
   <si>
     <t>Name</t>
   </si>
@@ -116,7 +116,7 @@
     <t>CAP CER 0.1UF 6.3V X7R 0603</t>
   </si>
   <si>
-    <t>C6, C101, C201, C202, C402, C403, C404, C405</t>
+    <t>C6, C101, C201, C202, C402, C403, C404, C405, C406</t>
   </si>
   <si>
     <t>KYOCERA AVX</t>
@@ -212,19 +212,19 @@
     <t>1206</t>
   </si>
   <si>
-    <t>10164359-00011LF</t>
-  </si>
-  <si>
-    <t>USB TYPE C RECEPTACLE RIGHT ANGL</t>
+    <t>USB4125-GF-A</t>
+  </si>
+  <si>
+    <t>CONN RCPT TYPE C 6P SMD RA</t>
   </si>
   <si>
     <t>J1</t>
   </si>
   <si>
-    <t>Amphenol ICC (FCI)</t>
-  </si>
-  <si>
-    <t>609-10164359-00011LFCT-ND</t>
+    <t>GCT</t>
+  </si>
+  <si>
+    <t>2073-USB4125-GF-ACT-ND</t>
   </si>
   <si>
     <t>0530480210</t>
@@ -323,7 +323,10 @@
     <t>Panasonic Electronic Components</t>
   </si>
   <si>
-    <t>P470HCT-ND</t>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>667-ERJ-3EKF4700V</t>
   </si>
   <si>
     <t>470</t>
@@ -398,7 +401,7 @@
     <t>R215, R216, R301, R303, R402, R404</t>
   </si>
   <si>
-    <t>P10.0KHCT-ND</t>
+    <t>667-ERJ-3EKF1002V</t>
   </si>
   <si>
     <t>10k</t>
@@ -485,10 +488,10 @@
     <t>TDK InvenSense</t>
   </si>
   <si>
-    <t>1428-ICM-42670-PCT-ND</t>
-  </si>
-  <si>
-    <t>14-VFLGA</t>
+    <t>410-ICM-42670-P</t>
+  </si>
+  <si>
+    <t>LGA-14</t>
   </si>
   <si>
     <t>MC74HC244ADTR2G</t>
@@ -935,7 +938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1338B1-C7CC-467C-88F0-7C518FEC3836}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359627E5-9883-4B82-BC93-CDBE6EE2AB2A}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1054,7 +1057,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>27</v>
@@ -1425,13 +1428,13 @@
         <v>91</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>17</v>
@@ -1439,13 +1442,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1454,16 +1457,16 @@
         <v>94</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>17</v>
@@ -1471,13 +1474,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>
@@ -1486,16 +1489,16 @@
         <v>88</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>17</v>
@@ -1503,13 +1506,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -1518,16 +1521,16 @@
         <v>94</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>17</v>
@@ -1535,13 +1538,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D20" s="1">
         <v>14</v>
@@ -1550,16 +1553,16 @@
         <v>94</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>17</v>
@@ -1567,13 +1570,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D21" s="1">
         <v>6</v>
@@ -1582,16 +1585,16 @@
         <v>94</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>17</v>
@@ -1599,13 +1602,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
@@ -1614,178 +1617,178 @@
         <v>88</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
@@ -1794,47 +1797,47 @@
         <v>49</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>